<commit_message>
Deploying to gh-pages from  @ fbd649da55088fbbdf6efeadbaddfe5762fa8c8f 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/17.4.1.xlsx
+++ b/en/downloads/data-excel/17.4.1.xlsx
@@ -479,18 +479,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="21" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +513,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -538,7 +537,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -558,8 +557,10 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -617,8 +618,14 @@
       <c r="S4" s="6">
         <v>2022</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T4" s="6">
+        <v>2023</v>
+      </c>
+      <c r="U4" s="6">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -676,8 +683,14 @@
       <c r="S5" s="8">
         <v>10.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="8">
+        <v>10.8</v>
+      </c>
+      <c r="U5" s="8">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -701,7 +714,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -719,7 +732,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -737,7 +750,7 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -755,7 +768,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -773,7 +786,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -791,7 +804,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -809,7 +822,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -827,7 +840,7 @@
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -845,7 +858,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>

</xml_diff>